<commit_message>
Changed the excel sheet
</commit_message>
<xml_diff>
--- a/Assignment3/Speeds of the sort algorithms.xlsx
+++ b/Assignment3/Speeds of the sort algorithms.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HvA\Programming\algorithms_and_data_structures\Assignment3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juacq\HvA\Programming\algorithms_and_data_structures\Assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93462A5-C0AA-4D97-9D74-66A21ECCC451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3117B9-FFCF-41CB-9971-7C5B44B2DF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7272825-25FB-4C2E-A03B-1298757C8EBB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F7272825-25FB-4C2E-A03B-1298757C8EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="39">
   <si>
     <t>The specifications of the device:</t>
   </si>
@@ -147,13 +147,16 @@
   <si>
     <t>Archer amount:</t>
   </si>
+  <si>
+    <t>GTX 1650</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -203,7 +206,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -522,7 +525,7 @@
   <dimension ref="A1:BN41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,6 +1814,9 @@
       </c>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
       <c r="F14" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>